<commit_message>
Final Data Collection over set of values
</commit_message>
<xml_diff>
--- a/optimize_processing/SamplingData1.xlsx
+++ b/optimize_processing/SamplingData1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="3435" firstSheet="5" activeTab="6"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14370" windowHeight="3435" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="BaseLine" sheetId="1" r:id="rId1"/>
@@ -1366,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O31"/>
+  <dimension ref="A2:O61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2782,6 +2782,1416 @@
       </c>
       <c r="O31">
         <v>93.689491586000045</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>50</v>
+      </c>
+      <c r="B32">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <v>0.97</v>
+      </c>
+      <c r="D32">
+        <v>26</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>22</v>
+      </c>
+      <c r="G32">
+        <v>2380</v>
+      </c>
+      <c r="H32">
+        <v>2380</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>1.366273002893704E-2</v>
+      </c>
+      <c r="K32">
+        <v>6.6692643921291345E-2</v>
+      </c>
+      <c r="L32">
+        <v>9.1631310357917634E-2</v>
+      </c>
+      <c r="M32">
+        <v>25</v>
+      </c>
+      <c r="N32">
+        <v>184.58363831089721</v>
+      </c>
+      <c r="O32">
+        <v>80.978181979538832</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>0.97</v>
+      </c>
+      <c r="D33">
+        <v>26</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>22</v>
+      </c>
+      <c r="G33">
+        <v>2380</v>
+      </c>
+      <c r="H33">
+        <v>2380</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>2.3535967698117477</v>
+      </c>
+      <c r="K33">
+        <v>2.2984358682915276</v>
+      </c>
+      <c r="L33">
+        <v>2.6118589412403712</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>186.50986080707267</v>
+      </c>
+      <c r="O33">
+        <v>7.4212810748089542</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>50</v>
+      </c>
+      <c r="B34">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>0.97</v>
+      </c>
+      <c r="D34">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <v>22</v>
+      </c>
+      <c r="G34">
+        <v>2380</v>
+      </c>
+      <c r="H34">
+        <v>2380</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34">
+        <v>6.0381297015602037E-3</v>
+      </c>
+      <c r="K34">
+        <v>9.4607030934551223E-2</v>
+      </c>
+      <c r="L34">
+        <v>8.0453584065583686E-2</v>
+      </c>
+      <c r="M34">
+        <v>47</v>
+      </c>
+      <c r="N34">
+        <v>182.73279799759237</v>
+      </c>
+      <c r="O34">
+        <v>152.23264465354509</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>50</v>
+      </c>
+      <c r="B35">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>0.97</v>
+      </c>
+      <c r="D35">
+        <v>26</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>22</v>
+      </c>
+      <c r="G35">
+        <v>2380</v>
+      </c>
+      <c r="H35">
+        <v>2380</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
+        <v>1.3338350313405207E-7</v>
+      </c>
+      <c r="K35">
+        <v>5.5867372113554685E-2</v>
+      </c>
+      <c r="L35">
+        <v>3.7877324012182981E-2</v>
+      </c>
+      <c r="M35">
+        <v>84</v>
+      </c>
+      <c r="N35">
+        <v>183.11340154527332</v>
+      </c>
+      <c r="O35">
+        <v>261.74544133503503</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>25</v>
+      </c>
+      <c r="C36">
+        <v>0.97</v>
+      </c>
+      <c r="D36">
+        <v>26</v>
+      </c>
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>22</v>
+      </c>
+      <c r="G36">
+        <v>2380</v>
+      </c>
+      <c r="H36">
+        <v>2380</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36">
+        <v>3.6238843896093141E-4</v>
+      </c>
+      <c r="K36">
+        <v>7.6817691142946495E-2</v>
+      </c>
+      <c r="L36">
+        <v>3.9043249517902792E-2</v>
+      </c>
+      <c r="M36">
+        <v>46</v>
+      </c>
+      <c r="N36">
+        <v>183.15789969367412</v>
+      </c>
+      <c r="O36">
+        <v>149.29928924430362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>0.97</v>
+      </c>
+      <c r="D37">
+        <v>26</v>
+      </c>
+      <c r="E37">
+        <v>20</v>
+      </c>
+      <c r="F37">
+        <v>22</v>
+      </c>
+      <c r="G37">
+        <v>2380</v>
+      </c>
+      <c r="H37">
+        <v>2380</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>5.8841550973502318E-5</v>
+      </c>
+      <c r="K37">
+        <v>3.8901992545799353E-2</v>
+      </c>
+      <c r="L37">
+        <v>0.10028153063632129</v>
+      </c>
+      <c r="M37">
+        <v>55</v>
+      </c>
+      <c r="N37">
+        <v>186.83642355799242</v>
+      </c>
+      <c r="O37">
+        <v>171.25738919081434</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>50</v>
+      </c>
+      <c r="B38">
+        <v>25</v>
+      </c>
+      <c r="C38">
+        <v>0.97</v>
+      </c>
+      <c r="D38">
+        <v>26</v>
+      </c>
+      <c r="E38">
+        <v>20</v>
+      </c>
+      <c r="F38">
+        <v>22</v>
+      </c>
+      <c r="G38">
+        <v>2380</v>
+      </c>
+      <c r="H38">
+        <v>2380</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <v>2.1574312175245284E-3</v>
+      </c>
+      <c r="K38">
+        <v>7.7896999840753767E-2</v>
+      </c>
+      <c r="L38">
+        <v>8.716858775528584E-2</v>
+      </c>
+      <c r="M38">
+        <v>52</v>
+      </c>
+      <c r="N38">
+        <v>183.17131488294535</v>
+      </c>
+      <c r="O38">
+        <v>165.94508139912557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>0.97</v>
+      </c>
+      <c r="D39">
+        <v>26</v>
+      </c>
+      <c r="E39">
+        <v>20</v>
+      </c>
+      <c r="F39">
+        <v>22</v>
+      </c>
+      <c r="G39">
+        <v>2380</v>
+      </c>
+      <c r="H39">
+        <v>2380</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39">
+        <v>6.6971618032837703E-3</v>
+      </c>
+      <c r="K39">
+        <v>7.6798603473640287E-2</v>
+      </c>
+      <c r="L39">
+        <v>0.11560536447582104</v>
+      </c>
+      <c r="M39">
+        <v>25</v>
+      </c>
+      <c r="N39">
+        <v>183.05129780983648</v>
+      </c>
+      <c r="O39">
+        <v>79.850808618176941</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>50</v>
+      </c>
+      <c r="B40">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <v>0.97</v>
+      </c>
+      <c r="D40">
+        <v>26</v>
+      </c>
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>22</v>
+      </c>
+      <c r="G40">
+        <v>2380</v>
+      </c>
+      <c r="H40">
+        <v>2380</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>6.8239072186986093E-3</v>
+      </c>
+      <c r="K40">
+        <v>6.9542121096911338E-2</v>
+      </c>
+      <c r="L40">
+        <v>9.5235295835321726E-2</v>
+      </c>
+      <c r="M40">
+        <v>29</v>
+      </c>
+      <c r="N40">
+        <v>183.64838934415837</v>
+      </c>
+      <c r="O40">
+        <v>93.744397206964962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>25</v>
+      </c>
+      <c r="C41">
+        <v>0.97</v>
+      </c>
+      <c r="D41">
+        <v>26</v>
+      </c>
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="F41">
+        <v>22</v>
+      </c>
+      <c r="G41">
+        <v>2380</v>
+      </c>
+      <c r="H41">
+        <v>2380</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>1.7598650017005269E-2</v>
+      </c>
+      <c r="K41">
+        <v>9.0153938570145489E-2</v>
+      </c>
+      <c r="L41">
+        <v>8.992773703606223E-2</v>
+      </c>
+      <c r="M41">
+        <v>31</v>
+      </c>
+      <c r="N41">
+        <v>183.18809488736457</v>
+      </c>
+      <c r="O41">
+        <v>98.933058078756048</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>50</v>
+      </c>
+      <c r="B42">
+        <v>25</v>
+      </c>
+      <c r="C42">
+        <v>0.97</v>
+      </c>
+      <c r="D42">
+        <v>26</v>
+      </c>
+      <c r="E42">
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <v>22</v>
+      </c>
+      <c r="G42">
+        <v>2380</v>
+      </c>
+      <c r="H42">
+        <v>4760</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42">
+        <v>1.494105991154586</v>
+      </c>
+      <c r="K42">
+        <v>1.6079086881951579</v>
+      </c>
+      <c r="L42">
+        <v>1.4692837763289257</v>
+      </c>
+      <c r="M42">
+        <v>30</v>
+      </c>
+      <c r="N42">
+        <v>183.163463848839</v>
+      </c>
+      <c r="O42">
+        <v>188.15540634361383</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>50</v>
+      </c>
+      <c r="B43">
+        <v>25</v>
+      </c>
+      <c r="C43">
+        <v>0.97</v>
+      </c>
+      <c r="D43">
+        <v>26</v>
+      </c>
+      <c r="E43">
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <v>2380</v>
+      </c>
+      <c r="H43">
+        <v>4760</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>1.1553790370436913E-2</v>
+      </c>
+      <c r="K43">
+        <v>4.5851181501723855E-2</v>
+      </c>
+      <c r="L43">
+        <v>7.0549565577578674E-2</v>
+      </c>
+      <c r="M43">
+        <v>58</v>
+      </c>
+      <c r="N43">
+        <v>183.20903178327052</v>
+      </c>
+      <c r="O43">
+        <v>362.63523858281121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>50</v>
+      </c>
+      <c r="B44">
+        <v>25</v>
+      </c>
+      <c r="C44">
+        <v>0.97</v>
+      </c>
+      <c r="D44">
+        <v>26</v>
+      </c>
+      <c r="E44">
+        <v>20</v>
+      </c>
+      <c r="F44">
+        <v>22</v>
+      </c>
+      <c r="G44">
+        <v>2380</v>
+      </c>
+      <c r="H44">
+        <v>4760</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+      <c r="J44">
+        <v>1.557911524635182</v>
+      </c>
+      <c r="K44">
+        <v>1.2786146758028847</v>
+      </c>
+      <c r="L44">
+        <v>1.7164601488959106</v>
+      </c>
+      <c r="M44">
+        <v>23</v>
+      </c>
+      <c r="N44">
+        <v>178.4815984124665</v>
+      </c>
+      <c r="O44">
+        <v>141.4959143470864</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>50</v>
+      </c>
+      <c r="B45">
+        <v>25</v>
+      </c>
+      <c r="C45">
+        <v>0.97</v>
+      </c>
+      <c r="D45">
+        <v>26</v>
+      </c>
+      <c r="E45">
+        <v>20</v>
+      </c>
+      <c r="F45">
+        <v>22</v>
+      </c>
+      <c r="G45">
+        <v>2380</v>
+      </c>
+      <c r="H45">
+        <v>4760</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>2.5910892012149743E-5</v>
+      </c>
+      <c r="K45">
+        <v>8.6742557013077801E-2</v>
+      </c>
+      <c r="L45">
+        <v>8.9619254131656084E-2</v>
+      </c>
+      <c r="M45">
+        <v>59</v>
+      </c>
+      <c r="N45">
+        <v>183.43958999182567</v>
+      </c>
+      <c r="O45">
+        <v>368.57329362487218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>50</v>
+      </c>
+      <c r="B46">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>0.97</v>
+      </c>
+      <c r="D46">
+        <v>26</v>
+      </c>
+      <c r="E46">
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <v>22</v>
+      </c>
+      <c r="G46">
+        <v>2380</v>
+      </c>
+      <c r="H46">
+        <v>4760</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <v>7.1254967700253692E-3</v>
+      </c>
+      <c r="K46">
+        <v>0.15566846682902866</v>
+      </c>
+      <c r="L46">
+        <v>0.10688283358235008</v>
+      </c>
+      <c r="M46">
+        <v>34</v>
+      </c>
+      <c r="N46">
+        <v>183.95215122379417</v>
+      </c>
+      <c r="O46">
+        <v>219.19810601990091</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>0.97</v>
+      </c>
+      <c r="D47">
+        <v>26</v>
+      </c>
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <v>22</v>
+      </c>
+      <c r="G47">
+        <v>2380</v>
+      </c>
+      <c r="H47">
+        <v>4760</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>3.4698050066159572E-4</v>
+      </c>
+      <c r="K47">
+        <v>0.11474785814937384</v>
+      </c>
+      <c r="L47">
+        <v>0.13147310382298608</v>
+      </c>
+      <c r="M47">
+        <v>43</v>
+      </c>
+      <c r="N47">
+        <v>183.80279895146481</v>
+      </c>
+      <c r="O47">
+        <v>275.35624116309651</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <v>0.97</v>
+      </c>
+      <c r="D48">
+        <v>26</v>
+      </c>
+      <c r="E48">
+        <v>20</v>
+      </c>
+      <c r="F48">
+        <v>22</v>
+      </c>
+      <c r="G48">
+        <v>2380</v>
+      </c>
+      <c r="H48">
+        <v>4760</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>6.2936249549410857E-3</v>
+      </c>
+      <c r="K48">
+        <v>0.10005320612485613</v>
+      </c>
+      <c r="L48">
+        <v>9.7131136773275686E-2</v>
+      </c>
+      <c r="M48">
+        <v>35</v>
+      </c>
+      <c r="N48">
+        <v>183.92748184925676</v>
+      </c>
+      <c r="O48">
+        <v>222.5370494914894</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <v>0.97</v>
+      </c>
+      <c r="D49">
+        <v>26</v>
+      </c>
+      <c r="E49">
+        <v>20</v>
+      </c>
+      <c r="F49">
+        <v>22</v>
+      </c>
+      <c r="G49">
+        <v>2380</v>
+      </c>
+      <c r="H49">
+        <v>4760</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>0.8742306856938713</v>
+      </c>
+      <c r="K49">
+        <v>0.94822953808358035</v>
+      </c>
+      <c r="L49">
+        <v>0.89419761863723379</v>
+      </c>
+      <c r="M49">
+        <v>48</v>
+      </c>
+      <c r="N49">
+        <v>184.18859748153531</v>
+      </c>
+      <c r="O49">
+        <v>303.55798336881173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>25</v>
+      </c>
+      <c r="C50">
+        <v>0.97</v>
+      </c>
+      <c r="D50">
+        <v>26</v>
+      </c>
+      <c r="E50">
+        <v>20</v>
+      </c>
+      <c r="F50">
+        <v>22</v>
+      </c>
+      <c r="G50">
+        <v>2380</v>
+      </c>
+      <c r="H50">
+        <v>4760</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>1.518741189561118</v>
+      </c>
+      <c r="K50">
+        <v>1.3940462461294012</v>
+      </c>
+      <c r="L50">
+        <v>1.6954966172582038</v>
+      </c>
+      <c r="M50">
+        <v>20</v>
+      </c>
+      <c r="N50">
+        <v>184.08945693266023</v>
+      </c>
+      <c r="O50">
+        <v>129.10761310934637</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>25</v>
+      </c>
+      <c r="C51">
+        <v>0.97</v>
+      </c>
+      <c r="D51">
+        <v>26</v>
+      </c>
+      <c r="E51">
+        <v>20</v>
+      </c>
+      <c r="F51">
+        <v>22</v>
+      </c>
+      <c r="G51">
+        <v>2380</v>
+      </c>
+      <c r="H51">
+        <v>4760</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>3.1079761473666217E-3</v>
+      </c>
+      <c r="K51">
+        <v>7.0912598225917278E-2</v>
+      </c>
+      <c r="L51">
+        <v>8.8717882488785732E-2</v>
+      </c>
+      <c r="M51">
+        <v>45</v>
+      </c>
+      <c r="N51">
+        <v>183.82439872833109</v>
+      </c>
+      <c r="O51">
+        <v>282.2467510984626</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <v>0.97</v>
+      </c>
+      <c r="D52">
+        <v>26</v>
+      </c>
+      <c r="E52">
+        <v>20</v>
+      </c>
+      <c r="F52">
+        <v>22</v>
+      </c>
+      <c r="G52">
+        <v>2380</v>
+      </c>
+      <c r="H52">
+        <v>7140</v>
+      </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
+      <c r="J52">
+        <v>1.8374258141780748E-2</v>
+      </c>
+      <c r="K52">
+        <v>0.12545192929931043</v>
+      </c>
+      <c r="L52">
+        <v>6.4931197956281217E-2</v>
+      </c>
+      <c r="M52">
+        <v>38</v>
+      </c>
+      <c r="N52">
+        <v>183.91329541187366</v>
+      </c>
+      <c r="O52">
+        <v>357.90538098751153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>25</v>
+      </c>
+      <c r="C53">
+        <v>0.97</v>
+      </c>
+      <c r="D53">
+        <v>26</v>
+      </c>
+      <c r="E53">
+        <v>20</v>
+      </c>
+      <c r="F53">
+        <v>22</v>
+      </c>
+      <c r="G53">
+        <v>2380</v>
+      </c>
+      <c r="H53">
+        <v>7140</v>
+      </c>
+      <c r="I53">
+        <v>3</v>
+      </c>
+      <c r="J53">
+        <v>2.2607960424558362</v>
+      </c>
+      <c r="K53">
+        <v>2.6379775306552595</v>
+      </c>
+      <c r="L53">
+        <v>2.7163332989414144</v>
+      </c>
+      <c r="M53">
+        <v>14</v>
+      </c>
+      <c r="N53">
+        <v>184.10958816860116</v>
+      </c>
+      <c r="O53">
+        <v>142.11038265980685</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <v>0.97</v>
+      </c>
+      <c r="D54">
+        <v>26</v>
+      </c>
+      <c r="E54">
+        <v>20</v>
+      </c>
+      <c r="F54">
+        <v>22</v>
+      </c>
+      <c r="G54">
+        <v>2380</v>
+      </c>
+      <c r="H54">
+        <v>7140</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="J54">
+        <v>0.94053176631366764</v>
+      </c>
+      <c r="K54">
+        <v>1.0185588818345011</v>
+      </c>
+      <c r="L54">
+        <v>0.63401740209598945</v>
+      </c>
+      <c r="M54">
+        <v>27</v>
+      </c>
+      <c r="N54">
+        <v>187.35723457896191</v>
+      </c>
+      <c r="O54">
+        <v>263.37191847892365</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>50</v>
+      </c>
+      <c r="B55">
+        <v>25</v>
+      </c>
+      <c r="C55">
+        <v>0.97</v>
+      </c>
+      <c r="D55">
+        <v>26</v>
+      </c>
+      <c r="E55">
+        <v>20</v>
+      </c>
+      <c r="F55">
+        <v>22</v>
+      </c>
+      <c r="G55">
+        <v>2380</v>
+      </c>
+      <c r="H55">
+        <v>7140</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>1.5242344512774213</v>
+      </c>
+      <c r="K55">
+        <v>1.7004438939897475</v>
+      </c>
+      <c r="L55">
+        <v>1.3346310338144127</v>
+      </c>
+      <c r="M55">
+        <v>30</v>
+      </c>
+      <c r="N55">
+        <v>185.28028665677377</v>
+      </c>
+      <c r="O55">
+        <v>275.31006226734269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>50</v>
+      </c>
+      <c r="B56">
+        <v>25</v>
+      </c>
+      <c r="C56">
+        <v>0.97</v>
+      </c>
+      <c r="D56">
+        <v>26</v>
+      </c>
+      <c r="E56">
+        <v>20</v>
+      </c>
+      <c r="F56">
+        <v>22</v>
+      </c>
+      <c r="G56">
+        <v>2380</v>
+      </c>
+      <c r="H56">
+        <v>7140</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <v>9.5600859311663609</v>
+      </c>
+      <c r="K56">
+        <v>9.7683524417692134</v>
+      </c>
+      <c r="L56">
+        <v>9.8242479833726044</v>
+      </c>
+      <c r="M56">
+        <v>25</v>
+      </c>
+      <c r="N56">
+        <v>184.94509679390197</v>
+      </c>
+      <c r="O56">
+        <v>249.28888901634019</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>50</v>
+      </c>
+      <c r="B57">
+        <v>25</v>
+      </c>
+      <c r="C57">
+        <v>0.97</v>
+      </c>
+      <c r="D57">
+        <v>26</v>
+      </c>
+      <c r="E57">
+        <v>20</v>
+      </c>
+      <c r="F57">
+        <v>22</v>
+      </c>
+      <c r="G57">
+        <v>2380</v>
+      </c>
+      <c r="H57">
+        <v>7140</v>
+      </c>
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <v>2.319973959961672</v>
+      </c>
+      <c r="K57">
+        <v>2.7163332988899858</v>
+      </c>
+      <c r="L57">
+        <v>2.3506730471163348</v>
+      </c>
+      <c r="M57">
+        <v>20</v>
+      </c>
+      <c r="N57">
+        <v>185.31986632504351</v>
+      </c>
+      <c r="O57">
+        <v>198.41227663990591</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>50</v>
+      </c>
+      <c r="B58">
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <v>0.97</v>
+      </c>
+      <c r="D58">
+        <v>26</v>
+      </c>
+      <c r="E58">
+        <v>20</v>
+      </c>
+      <c r="F58">
+        <v>22</v>
+      </c>
+      <c r="G58">
+        <v>2380</v>
+      </c>
+      <c r="H58">
+        <v>7140</v>
+      </c>
+      <c r="I58">
+        <v>3</v>
+      </c>
+      <c r="J58">
+        <v>2.4432575991379095</v>
+      </c>
+      <c r="K58">
+        <v>2.2984358682915276</v>
+      </c>
+      <c r="L58">
+        <v>2.193961510641913</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>184.19097884214378</v>
+      </c>
+      <c r="O58">
+        <v>19.986157681148221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>50</v>
+      </c>
+      <c r="B59">
+        <v>25</v>
+      </c>
+      <c r="C59">
+        <v>0.97</v>
+      </c>
+      <c r="D59">
+        <v>26</v>
+      </c>
+      <c r="E59">
+        <v>20</v>
+      </c>
+      <c r="F59">
+        <v>22</v>
+      </c>
+      <c r="G59">
+        <v>2380</v>
+      </c>
+      <c r="H59">
+        <v>7140</v>
+      </c>
+      <c r="I59">
+        <v>3</v>
+      </c>
+      <c r="J59">
+        <v>1.2701548527203489E-3</v>
+      </c>
+      <c r="K59">
+        <v>0.12700645659864251</v>
+      </c>
+      <c r="L59">
+        <v>0.10710975730659134</v>
+      </c>
+      <c r="M59">
+        <v>53</v>
+      </c>
+      <c r="N59">
+        <v>184.58929423100375</v>
+      </c>
+      <c r="O59">
+        <v>503.86538143426191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>50</v>
+      </c>
+      <c r="B60">
+        <v>25</v>
+      </c>
+      <c r="C60">
+        <v>0.97</v>
+      </c>
+      <c r="D60">
+        <v>26</v>
+      </c>
+      <c r="E60">
+        <v>20</v>
+      </c>
+      <c r="F60">
+        <v>22</v>
+      </c>
+      <c r="G60">
+        <v>2380</v>
+      </c>
+      <c r="H60">
+        <v>7140</v>
+      </c>
+      <c r="I60">
+        <v>3</v>
+      </c>
+      <c r="J60">
+        <v>1.2929207337272356E-2</v>
+      </c>
+      <c r="K60">
+        <v>0.16804424868919052</v>
+      </c>
+      <c r="L60">
+        <v>0.10272582800405085</v>
+      </c>
+      <c r="M60">
+        <v>60</v>
+      </c>
+      <c r="N60">
+        <v>184.06889766156365</v>
+      </c>
+      <c r="O60">
+        <v>560.99482916627926</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>50</v>
+      </c>
+      <c r="B61">
+        <v>25</v>
+      </c>
+      <c r="C61">
+        <v>0.97</v>
+      </c>
+      <c r="D61">
+        <v>26</v>
+      </c>
+      <c r="E61">
+        <v>20</v>
+      </c>
+      <c r="F61">
+        <v>22</v>
+      </c>
+      <c r="G61">
+        <v>2380</v>
+      </c>
+      <c r="H61">
+        <v>7140</v>
+      </c>
+      <c r="I61">
+        <v>3</v>
+      </c>
+      <c r="J61">
+        <v>1.5466761552534265</v>
+      </c>
+      <c r="K61">
+        <v>1.5572665803689556</v>
+      </c>
+      <c r="L61">
+        <v>1.4539871565231772</v>
+      </c>
+      <c r="M61">
+        <v>20</v>
+      </c>
+      <c r="N61">
+        <v>185.66233489856955</v>
+      </c>
+      <c r="O61">
+        <v>193.95990113534967</v>
       </c>
     </row>
   </sheetData>
@@ -8365,10 +9775,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O58"/>
+  <dimension ref="A2:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45:AI49"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10723,312 +12133,312 @@
         <v>8.9795732447238183</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64">
         <f>AVERAGE(A2:A11)</f>
         <v>50</v>
       </c>
-      <c r="B54">
-        <f t="shared" ref="B54:O54" si="0">AVERAGE(B2:B11)</f>
-        <v>25</v>
-      </c>
-      <c r="C54">
+      <c r="B64">
+        <f t="shared" ref="B64:O64" si="0">AVERAGE(B2:B11)</f>
+        <v>25</v>
+      </c>
+      <c r="C64">
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
-      <c r="D54">
+      <c r="D64">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="E54">
+      <c r="E64">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F54">
+      <c r="F64">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G54">
+      <c r="G64">
         <f t="shared" si="0"/>
         <v>1547</v>
       </c>
-      <c r="H54">
+      <c r="H64">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="I54">
+      <c r="I64">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J54">
+      <c r="J64">
         <f t="shared" si="0"/>
         <v>1.4464761566072323E-3</v>
       </c>
-      <c r="K54">
+      <c r="K64">
         <f t="shared" si="0"/>
         <v>2.0473697705505188E-2</v>
       </c>
-      <c r="L54">
+      <c r="L64">
         <f t="shared" si="0"/>
         <v>1.8817581619467744E-2</v>
       </c>
-      <c r="M54">
+      <c r="M64">
         <f t="shared" si="0"/>
         <v>36.799999999999997</v>
       </c>
-      <c r="N54">
+      <c r="N64">
         <f t="shared" si="0"/>
         <v>214.82435507961213</v>
       </c>
-      <c r="O54">
+      <c r="O64">
         <f t="shared" si="0"/>
         <v>4.1350252595076329</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65">
         <f>AVERAGE(A12:A21)</f>
         <v>50</v>
       </c>
-      <c r="B55">
-        <f t="shared" ref="B55:O55" si="1">AVERAGE(B12:B21)</f>
-        <v>25</v>
-      </c>
-      <c r="C55">
+      <c r="B65">
+        <f t="shared" ref="B65:O65" si="1">AVERAGE(B12:B21)</f>
+        <v>25</v>
+      </c>
+      <c r="C65">
         <f t="shared" si="1"/>
         <v>0.97</v>
       </c>
-      <c r="D55">
+      <c r="D65">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="E55">
+      <c r="E65">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F55">
+      <c r="F65">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="G55">
+      <c r="G65">
         <f t="shared" si="1"/>
         <v>1785</v>
       </c>
-      <c r="H55">
+      <c r="H65">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="I55">
+      <c r="I65">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J55">
+      <c r="J65">
         <f t="shared" si="1"/>
         <v>2.5261837403124275E-4</v>
       </c>
-      <c r="K55">
+      <c r="K65">
         <f t="shared" si="1"/>
         <v>1.7990011982762823E-2</v>
       </c>
-      <c r="L55">
+      <c r="L65">
         <f t="shared" si="1"/>
         <v>2.5005880174614508E-2</v>
       </c>
-      <c r="M55">
+      <c r="M65">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="N55">
+      <c r="N65">
         <f t="shared" si="1"/>
         <v>214.80317228988542</v>
       </c>
-      <c r="O55">
+      <c r="O65">
         <f t="shared" si="1"/>
         <v>5.0788869697405108</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66">
         <f>AVERAGE(A22:A31)</f>
         <v>50</v>
       </c>
-      <c r="B56">
-        <f t="shared" ref="B56:O56" si="2">AVERAGE(B22:B31)</f>
-        <v>25</v>
-      </c>
-      <c r="C56">
+      <c r="B66">
+        <f t="shared" ref="B66:O66" si="2">AVERAGE(B22:B31)</f>
+        <v>25</v>
+      </c>
+      <c r="C66">
         <f t="shared" si="2"/>
         <v>0.97</v>
       </c>
-      <c r="D56">
+      <c r="D66">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="E56">
+      <c r="E66">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="F56">
+      <c r="F66">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="G56">
+      <c r="G66">
         <f t="shared" si="2"/>
         <v>2142</v>
       </c>
-      <c r="H56">
+      <c r="H66">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="I56">
+      <c r="I66">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J56">
+      <c r="J66">
         <f t="shared" si="2"/>
         <v>4.6831586438029978E-4</v>
       </c>
-      <c r="K56">
+      <c r="K66">
         <f t="shared" si="2"/>
         <v>2.1539265590598194E-2</v>
       </c>
-      <c r="L56">
+      <c r="L66">
         <f t="shared" si="2"/>
         <v>2.5361387587458852E-2</v>
       </c>
-      <c r="M56">
+      <c r="M66">
         <f t="shared" si="2"/>
         <v>40.799999999999997</v>
       </c>
-      <c r="N56">
+      <c r="N66">
         <f t="shared" si="2"/>
         <v>219.48566637648014</v>
       </c>
-      <c r="O56">
+      <c r="O66">
         <f t="shared" si="2"/>
         <v>5.9705460798862111</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67">
         <f>AVERAGE(A32:A41)</f>
         <v>50</v>
       </c>
-      <c r="B57">
-        <f t="shared" ref="B57:O57" si="3">AVERAGE(B32:B41)</f>
-        <v>25</v>
-      </c>
-      <c r="C57">
+      <c r="B67">
+        <f t="shared" ref="B67:O67" si="3">AVERAGE(B32:B41)</f>
+        <v>25</v>
+      </c>
+      <c r="C67">
         <f t="shared" si="3"/>
         <v>0.97</v>
       </c>
-      <c r="D57">
+      <c r="D67">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="E57">
+      <c r="E67">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="F57">
+      <c r="F67">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="G57">
+      <c r="G67">
         <f t="shared" si="3"/>
         <v>2975</v>
       </c>
-      <c r="H57">
+      <c r="H67">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="I57">
+      <c r="I67">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="J57">
+      <c r="J67">
         <f t="shared" si="3"/>
         <v>8.5887250967488935E-2</v>
       </c>
-      <c r="K57">
+      <c r="K67">
         <f t="shared" si="3"/>
         <v>0.11431187110655758</v>
       </c>
-      <c r="L57">
+      <c r="L67">
         <f t="shared" si="3"/>
         <v>9.3979450546906401E-2</v>
       </c>
-      <c r="M57">
+      <c r="M67">
         <f t="shared" si="3"/>
         <v>45.6</v>
       </c>
-      <c r="N57">
+      <c r="N67">
         <f t="shared" si="3"/>
         <v>231.09534425738616</v>
       </c>
-      <c r="O57">
+      <c r="O67">
         <f t="shared" si="3"/>
         <v>8.7436332336395797</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68">
         <f>AVERAGE(A42:A51)</f>
         <v>50</v>
       </c>
-      <c r="B58">
-        <f t="shared" ref="B58:O58" si="4">AVERAGE(B42:B51)</f>
-        <v>25</v>
-      </c>
-      <c r="C58">
+      <c r="B68">
+        <f t="shared" ref="B68:O68" si="4">AVERAGE(B42:B51)</f>
+        <v>25</v>
+      </c>
+      <c r="C68">
         <f t="shared" si="4"/>
         <v>0.97</v>
       </c>
-      <c r="D58">
+      <c r="D68">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="E58">
+      <c r="E68">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="F58">
+      <c r="F68">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="G58">
+      <c r="G68">
         <f t="shared" si="4"/>
         <v>2975</v>
       </c>
-      <c r="H58">
+      <c r="H68">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="I58">
+      <c r="I68">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="J58">
+      <c r="J68">
         <f t="shared" si="4"/>
         <v>8.5887250967488935E-2</v>
       </c>
-      <c r="K58">
+      <c r="K68">
         <f t="shared" si="4"/>
         <v>0.11431187110655758</v>
       </c>
-      <c r="L58">
+      <c r="L68">
         <f t="shared" si="4"/>
         <v>9.3979450546906401E-2</v>
       </c>
-      <c r="M58">
+      <c r="M68">
         <f t="shared" si="4"/>
         <v>45.6</v>
       </c>
-      <c r="N58">
+      <c r="N68">
         <f t="shared" si="4"/>
         <v>231.09534425738616</v>
       </c>
-      <c r="O58">
+      <c r="O68">
         <f t="shared" si="4"/>
         <v>8.7436332336395797</v>
       </c>

</xml_diff>